<commit_message>
✨ driver script 버그, 플롯 수정
</commit_message>
<xml_diff>
--- a/AssetSelling/asset_selling_policy_parameters.xlsx
+++ b/AssetSelling/asset_selling_policy_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnascime/Dropbox/PythonProjects/ORF411/github_private/seqdecisionlib_Asset/Asset selling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongjun-u/Documents/GitHub/IIE4124-Optimization-Theory-and-Application/AssetSelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15C2239-7512-A040-BCCB-1AB3553C23EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01DABDB-2624-3C41-844C-3FA812AAFBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="4440" windowWidth="17740" windowHeight="8960" activeTab="3" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
+    <workbookView xWindow="-940" yWindow="-19600" windowWidth="25060" windowHeight="17000" activeTab="4" xr2:uid="{1DA193D8-6EE7-6A44-BDCF-D14F5A013405}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>After setting up the parameters and saving this spreadsheet, just run  'AssetSellingDriverScript'</t>
   </si>
   <si>
-    <t>TimeHorizon</t>
-  </si>
-  <si>
     <t>InitialPrice</t>
   </si>
   <si>
@@ -141,7 +138,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -151,7 +148,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -167,7 +164,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -177,7 +174,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -193,16 +190,20 @@
   <si>
     <t>DiscountFactor</t>
   </si>
+  <si>
+    <t>TimeHorizon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -210,8 +211,15 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -246,7 +254,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -262,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -302,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -408,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,23 +569,23 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="73.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17">
+    <row r="1" spans="1:2" ht="19">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -585,15 +593,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17">
+    <row r="3" spans="1:2" ht="19">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="19">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -601,41 +609,42 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="68">
+    <row r="5" spans="1:2" ht="76">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="51">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="57">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="51">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="57">
       <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="38">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="34">
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="34">
+    <row r="9" spans="1:2" ht="38">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -646,10 +655,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -693,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -723,6 +732,7 @@
       <c r="E8" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -735,9 +745,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18"/>
   <cols>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -775,6 +785,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -783,13 +794,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B272AC-B9F0-6245-988D-8924FC3BFAF0}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="5" width="13.1640625" customWidth="1"/>
+    <col min="2" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -797,25 +808,25 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
@@ -829,7 +840,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>0.99</v>
@@ -838,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -850,13 +861,14 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="J2">
-        <v>40</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -865,26 +877,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7AFC32-A488-924F-BA5B-5E75A4CE45E5}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0.9</v>
@@ -898,7 +910,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -912,7 +924,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -925,6 +937,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>